<commit_message>
Updated for less effort
</commit_message>
<xml_diff>
--- a/data/covid-19-pandas-output-scandi.xlsx
+++ b/data/covid-19-pandas-output-scandi.xlsx
@@ -402,7 +402,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G35"/>
+  <dimension ref="A1:G41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1213,6 +1213,144 @@
         <v>3315</v>
       </c>
     </row>
+    <row r="36" spans="1:7">
+      <c r="A36" s="2">
+        <v>43938</v>
+      </c>
+      <c r="B36">
+        <v>14576</v>
+      </c>
+      <c r="C36">
+        <v>1400</v>
+      </c>
+      <c r="D36">
+        <v>161</v>
+      </c>
+      <c r="E36">
+        <v>336</v>
+      </c>
+      <c r="F36">
+        <v>82</v>
+      </c>
+      <c r="G36">
+        <v>3459</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7">
+      <c r="A37" s="2">
+        <v>43939</v>
+      </c>
+      <c r="B37">
+        <v>15464</v>
+      </c>
+      <c r="C37">
+        <v>1511</v>
+      </c>
+      <c r="D37">
+        <v>164</v>
+      </c>
+      <c r="E37">
+        <v>346</v>
+      </c>
+      <c r="F37">
+        <v>90</v>
+      </c>
+      <c r="G37">
+        <v>3601</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7">
+      <c r="A38" s="2">
+        <v>43940</v>
+      </c>
+      <c r="B38">
+        <v>16060</v>
+      </c>
+      <c r="C38">
+        <v>1540</v>
+      </c>
+      <c r="D38">
+        <v>165</v>
+      </c>
+      <c r="E38">
+        <v>355</v>
+      </c>
+      <c r="F38">
+        <v>94</v>
+      </c>
+      <c r="G38">
+        <v>3684</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7">
+      <c r="A39" s="2">
+        <v>43941</v>
+      </c>
+      <c r="B39">
+        <v>16509</v>
+      </c>
+      <c r="C39">
+        <v>1580</v>
+      </c>
+      <c r="D39">
+        <v>181</v>
+      </c>
+      <c r="E39">
+        <v>364</v>
+      </c>
+      <c r="F39">
+        <v>98</v>
+      </c>
+      <c r="G39">
+        <v>3751</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7">
+      <c r="A40" s="2">
+        <v>43942</v>
+      </c>
+      <c r="B40">
+        <v>17337</v>
+      </c>
+      <c r="C40">
+        <v>1765</v>
+      </c>
+      <c r="D40">
+        <v>182</v>
+      </c>
+      <c r="E40">
+        <v>370</v>
+      </c>
+      <c r="F40">
+        <v>141</v>
+      </c>
+      <c r="G40">
+        <v>3916</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7">
+      <c r="A41" s="2">
+        <v>43943</v>
+      </c>
+      <c r="B41">
+        <v>18100</v>
+      </c>
+      <c r="C41">
+        <v>1937</v>
+      </c>
+      <c r="D41">
+        <v>187</v>
+      </c>
+      <c r="E41">
+        <v>384</v>
+      </c>
+      <c r="F41">
+        <v>149</v>
+      </c>
+      <c r="G41">
+        <v>4054</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1220,7 +1358,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G35"/>
+  <dimension ref="A1:G41"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2031,6 +2169,144 @@
         <v>9694.613532346933</v>
       </c>
     </row>
+    <row r="36" spans="1:7">
+      <c r="A36" s="2">
+        <v>43938</v>
+      </c>
+      <c r="B36">
+        <v>10792.21475571486</v>
+      </c>
+      <c r="C36">
+        <v>6974.618665215414</v>
+      </c>
+      <c r="D36">
+        <v>1496.599929464595</v>
+      </c>
+      <c r="E36">
+        <v>2910.664936207061</v>
+      </c>
+      <c r="F36">
+        <v>741.1211427581889</v>
+      </c>
+      <c r="G36">
+        <v>10115.73701610499</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7">
+      <c r="A37" s="2">
+        <v>43939</v>
+      </c>
+      <c r="B37">
+        <v>11449.69875016291</v>
+      </c>
+      <c r="C37">
+        <v>7527.606287957493</v>
+      </c>
+      <c r="D37">
+        <v>1524.48688467201</v>
+      </c>
+      <c r="E37">
+        <v>2997.291868832272</v>
+      </c>
+      <c r="F37">
+        <v>813.425644490695</v>
+      </c>
+      <c r="G37">
+        <v>10531.01156258863</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7">
+      <c r="A38" s="2">
+        <v>43940</v>
+      </c>
+      <c r="B38">
+        <v>11890.98305274291</v>
+      </c>
+      <c r="C38">
+        <v>7672.080531736955</v>
+      </c>
+      <c r="D38">
+        <v>1533.782536407814</v>
+      </c>
+      <c r="E38">
+        <v>3075.256108194961</v>
+      </c>
+      <c r="F38">
+        <v>849.5778953569481</v>
+      </c>
+      <c r="G38">
+        <v>10773.74245947695</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7">
+      <c r="A39" s="2">
+        <v>43941</v>
+      </c>
+      <c r="B39">
+        <v>12223.42709948522</v>
+      </c>
+      <c r="C39">
+        <v>7871.35535074311</v>
+      </c>
+      <c r="D39">
+        <v>1682.512964180693</v>
+      </c>
+      <c r="E39">
+        <v>3153.22034755765</v>
+      </c>
+      <c r="F39">
+        <v>885.7301462232012</v>
+      </c>
+      <c r="G39">
+        <v>10969.68185816994</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7">
+      <c r="A40" s="2">
+        <v>43942</v>
+      </c>
+      <c r="B40">
+        <v>12836.48649971381</v>
+      </c>
+      <c r="C40">
+        <v>8793.001388646575</v>
+      </c>
+      <c r="D40">
+        <v>1691.808615916498</v>
+      </c>
+      <c r="E40">
+        <v>3205.196507132776</v>
+      </c>
+      <c r="F40">
+        <v>1274.366843035422</v>
+      </c>
+      <c r="G40">
+        <v>11452.21918330938</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7">
+      <c r="A41" s="2">
+        <v>43943</v>
+      </c>
+      <c r="B41">
+        <v>13401.41925620465</v>
+      </c>
+      <c r="C41">
+        <v>9649.883110373041</v>
+      </c>
+      <c r="D41">
+        <v>1738.286874595523</v>
+      </c>
+      <c r="E41">
+        <v>3326.47421280807</v>
+      </c>
+      <c r="F41">
+        <v>1346.671344767929</v>
+      </c>
+      <c r="G41">
+        <v>11855.79585524418</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2038,7 +2314,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G35"/>
+  <dimension ref="A1:G41"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -2831,6 +3107,144 @@
         <v>181</v>
       </c>
     </row>
+    <row r="36" spans="1:7">
+      <c r="A36" s="2">
+        <v>43938</v>
+      </c>
+      <c r="B36">
+        <v>847</v>
+      </c>
+      <c r="C36">
+        <v>67</v>
+      </c>
+      <c r="D36">
+        <v>9</v>
+      </c>
+      <c r="E36">
+        <v>15</v>
+      </c>
+      <c r="F36">
+        <v>7</v>
+      </c>
+      <c r="G36">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7">
+      <c r="A37" s="2">
+        <v>43939</v>
+      </c>
+      <c r="B37">
+        <v>888</v>
+      </c>
+      <c r="C37">
+        <v>111</v>
+      </c>
+      <c r="D37">
+        <v>3</v>
+      </c>
+      <c r="E37">
+        <v>10</v>
+      </c>
+      <c r="F37">
+        <v>8</v>
+      </c>
+      <c r="G37">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7">
+      <c r="A38" s="2">
+        <v>43940</v>
+      </c>
+      <c r="B38">
+        <v>596</v>
+      </c>
+      <c r="C38">
+        <v>29</v>
+      </c>
+      <c r="D38">
+        <v>1</v>
+      </c>
+      <c r="E38">
+        <v>9</v>
+      </c>
+      <c r="F38">
+        <v>4</v>
+      </c>
+      <c r="G38">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7">
+      <c r="A39" s="2">
+        <v>43941</v>
+      </c>
+      <c r="B39">
+        <v>449</v>
+      </c>
+      <c r="C39">
+        <v>40</v>
+      </c>
+      <c r="D39">
+        <v>16</v>
+      </c>
+      <c r="E39">
+        <v>9</v>
+      </c>
+      <c r="F39">
+        <v>4</v>
+      </c>
+      <c r="G39">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7">
+      <c r="A40" s="2">
+        <v>43942</v>
+      </c>
+      <c r="B40">
+        <v>828</v>
+      </c>
+      <c r="C40">
+        <v>185</v>
+      </c>
+      <c r="D40">
+        <v>1</v>
+      </c>
+      <c r="E40">
+        <v>6</v>
+      </c>
+      <c r="F40">
+        <v>43</v>
+      </c>
+      <c r="G40">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7">
+      <c r="A41" s="2">
+        <v>43943</v>
+      </c>
+      <c r="B41">
+        <v>763</v>
+      </c>
+      <c r="C41">
+        <v>172</v>
+      </c>
+      <c r="D41">
+        <v>5</v>
+      </c>
+      <c r="E41">
+        <v>14</v>
+      </c>
+      <c r="F41">
+        <v>8</v>
+      </c>
+      <c r="G41">
+        <v>138</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2838,7 +3252,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G35"/>
+  <dimension ref="A1:G41"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3631,6 +4045,144 @@
         <v>529.3288233347798</v>
       </c>
     </row>
+    <row r="36" spans="1:7">
+      <c r="A36" s="2">
+        <v>43938</v>
+      </c>
+      <c r="B36">
+        <v>627.1271883980849</v>
+      </c>
+      <c r="C36">
+        <v>333.7853218353091</v>
+      </c>
+      <c r="D36">
+        <v>83.66086562224443</v>
+      </c>
+      <c r="E36">
+        <v>129.9403989378152</v>
+      </c>
+      <c r="F36">
+        <v>63.26643901594295</v>
+      </c>
+      <c r="G36">
+        <v>421.1234837580569</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7">
+      <c r="A37" s="2">
+        <v>43939</v>
+      </c>
+      <c r="B37">
+        <v>657.4839944480512</v>
+      </c>
+      <c r="C37">
+        <v>552.9876227420792</v>
+      </c>
+      <c r="D37">
+        <v>27.88695520741481</v>
+      </c>
+      <c r="E37">
+        <v>86.62693262521016</v>
+      </c>
+      <c r="F37">
+        <v>72.30450173250622</v>
+      </c>
+      <c r="G37">
+        <v>415.2745464836394</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7">
+      <c r="A38" s="2">
+        <v>43940</v>
+      </c>
+      <c r="B38">
+        <v>441.2843025799983</v>
+      </c>
+      <c r="C38">
+        <v>144.4742437794621</v>
+      </c>
+      <c r="D38">
+        <v>9.295651735804936</v>
+      </c>
+      <c r="E38">
+        <v>77.96423936268914</v>
+      </c>
+      <c r="F38">
+        <v>36.15225086625311</v>
+      </c>
+      <c r="G38">
+        <v>242.7308968883244</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7">
+      <c r="A39" s="2">
+        <v>43941</v>
+      </c>
+      <c r="B39">
+        <v>332.4440467423142</v>
+      </c>
+      <c r="C39">
+        <v>199.2748190061547</v>
+      </c>
+      <c r="D39">
+        <v>148.730427772879</v>
+      </c>
+      <c r="E39">
+        <v>77.96423936268914</v>
+      </c>
+      <c r="F39">
+        <v>36.15225086625311</v>
+      </c>
+      <c r="G39">
+        <v>195.9393986929848</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7">
+      <c r="A40" s="2">
+        <v>43942</v>
+      </c>
+      <c r="B40">
+        <v>613.0594002285883</v>
+      </c>
+      <c r="C40">
+        <v>921.6460379034654</v>
+      </c>
+      <c r="D40">
+        <v>9.295651735804936</v>
+      </c>
+      <c r="E40">
+        <v>51.97615957512609</v>
+      </c>
+      <c r="F40">
+        <v>388.636696812221</v>
+      </c>
+      <c r="G40">
+        <v>482.5373251394402</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7">
+      <c r="A41" s="2">
+        <v>43943</v>
+      </c>
+      <c r="B41">
+        <v>564.9327564908368</v>
+      </c>
+      <c r="C41">
+        <v>856.8817217264651</v>
+      </c>
+      <c r="D41">
+        <v>46.47825867902468</v>
+      </c>
+      <c r="E41">
+        <v>121.2777056752942</v>
+      </c>
+      <c r="F41">
+        <v>72.30450173250622</v>
+      </c>
+      <c r="G41">
+        <v>403.5766719348045</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3638,7 +4190,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G35"/>
+  <dimension ref="A1:G41"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -4359,6 +4911,144 @@
         <v>393.048584840853</v>
       </c>
     </row>
+    <row r="36" spans="1:7">
+      <c r="A36" s="2">
+        <v>43938</v>
+      </c>
+      <c r="B36">
+        <v>586.9969716198368</v>
+      </c>
+      <c r="C36">
+        <v>499.1834216104174</v>
+      </c>
+      <c r="D36">
+        <v>61.35130145631258</v>
+      </c>
+      <c r="E36">
+        <v>109.1499351077648</v>
+      </c>
+      <c r="F36">
+        <v>46.99792612612904</v>
+      </c>
+      <c r="G36">
+        <v>422.2932712129403</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7">
+      <c r="A37" s="2">
+        <v>43939</v>
+      </c>
+      <c r="B37">
+        <v>612.3189903249306</v>
+      </c>
+      <c r="C37">
+        <v>589.8534642582177</v>
+      </c>
+      <c r="D37">
+        <v>55.77391041482961</v>
+      </c>
+      <c r="E37">
+        <v>105.6848578027564</v>
+      </c>
+      <c r="F37">
+        <v>56.03598884269233</v>
+      </c>
+      <c r="G37">
+        <v>455.0473199496781</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7">
+      <c r="A38" s="2">
+        <v>43940</v>
+      </c>
+      <c r="B38">
+        <v>585.3680698317899</v>
+      </c>
+      <c r="C38">
+        <v>505.161666180602</v>
+      </c>
+      <c r="D38">
+        <v>48.33738902618567</v>
+      </c>
+      <c r="E38">
+        <v>97.02216454023539</v>
+      </c>
+      <c r="F38">
+        <v>54.22837629937967</v>
+      </c>
+      <c r="G38">
+        <v>432.2364645794501</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7">
+      <c r="A39" s="2">
+        <v>43941</v>
+      </c>
+      <c r="B39">
+        <v>539.1664918435484</v>
+      </c>
+      <c r="C39">
+        <v>375.6330338266014</v>
+      </c>
+      <c r="D39">
+        <v>57.63304076199059</v>
+      </c>
+      <c r="E39">
+        <v>95.28962588773119</v>
+      </c>
+      <c r="F39">
+        <v>46.99792612612904</v>
+      </c>
+      <c r="G39">
+        <v>360.8794298315571</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7">
+      <c r="A40" s="2">
+        <v>43942</v>
+      </c>
+      <c r="B40">
+        <v>534.2797864794076</v>
+      </c>
+      <c r="C40">
+        <v>430.4336090532939</v>
+      </c>
+      <c r="D40">
+        <v>55.77391041482961</v>
+      </c>
+      <c r="E40">
+        <v>84.89439397270598</v>
+      </c>
+      <c r="F40">
+        <v>119.3024278586353</v>
+      </c>
+      <c r="G40">
+        <v>351.5211301924892</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7">
+      <c r="A41" s="2">
+        <v>43943</v>
+      </c>
+      <c r="B41">
+        <v>521.840900097958</v>
+      </c>
+      <c r="C41">
+        <v>535.0528890315251</v>
+      </c>
+      <c r="D41">
+        <v>48.33738902618565</v>
+      </c>
+      <c r="E41">
+        <v>83.16185532020178</v>
+      </c>
+      <c r="F41">
+        <v>121.1100404019479</v>
+      </c>
+      <c r="G41">
+        <v>348.0117678278387</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>